<commit_message>
fix: incluir imagens ao dicionario da sapataria
</commit_message>
<xml_diff>
--- a/sapataria_dicionario.xlsx
+++ b/sapataria_dicionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alunos\repositories\modelagem_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD0143E-D1B1-4306-A00C-F9ADFB0D74C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131F1788-7B44-49F4-91B8-0263608807CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C402C656-23C7-49A2-859D-C12615F76A87}"/>
   </bookViews>
@@ -255,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -352,17 +352,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,14 +400,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,6 +421,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6978650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3020065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9A302F-CEB2-4657-997A-399C562AAC95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="10212" t="20433"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2254250" y="2997200"/>
+          <a:ext cx="6978650" cy="2893065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6635750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2665122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0999F9A5-5579-4544-A762-40C85CF15933}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="10539" t="5207"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1936750" y="6350"/>
+          <a:ext cx="6953250" cy="2658772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6981007-03C4-448A-AF72-A4C2E9F20287}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,575 +836,592 @@
     <col min="3" max="3" width="108.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="248" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" s="1">
-        <v>150</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E10" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E13" s="1">
-        <v>250</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="1">
-        <v>25</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E19" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="11">
-        <v>8</v>
+      <c r="E22" s="7">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="11">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E26" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="E27" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
+      <c r="E30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E31" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+      <c r="E34" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="E35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="E38" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
+      <c r="E39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E40" s="2">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A34:E34"/>
+  <mergeCells count="9">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>